<commit_message>
changes in the localT2 for the new HK genes and reactions
</commit_message>
<xml_diff>
--- a/Data/HK_G_acc_G_1.xlsx
+++ b/Data/HK_G_acc_G_1.xlsx
@@ -13,7 +13,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -69,247 +75,247 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>51.179673321234119</v>
+        <v>71.851851851851862</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>51.179673321234119</v>
+        <v>71.851851851851862</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>51.179673321234119</v>
+        <v>71.851851851851862</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>51.361161524500908</v>
+        <v>71.481481481481481</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>51.542649727767696</v>
+        <v>71.851851851851862</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>51.542649727767696</v>
+        <v>71.851851851851862</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>52.813067150635206</v>
+        <v>73.703703703703709</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>52.631578947368418</v>
+        <v>74.074074074074076</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>52.45009074410163</v>
+        <v>74.81481481481481</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>52.45009074410163</v>
+        <v>74.074074074074076</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>52.08711433756806</v>
+        <v>72.592592592592595</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>52.994555353901994</v>
+        <v>73.333333333333329</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>52.631578947368418</v>
+        <v>74.81481481481481</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>52.631578947368418</v>
+        <v>74.81481481481481</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>53.176043557168782</v>
+        <v>74.81481481481481</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>52.08711433756806</v>
+        <v>74.444444444444443</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>52.994555353901994</v>
+        <v>74.444444444444443</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>52.268602540834841</v>
+        <v>74.81481481481481</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>52.08711433756806</v>
+        <v>73.333333333333329</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>52.08711433756806</v>
+        <v>73.703703703703709</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>52.268602540834841</v>
+        <v>74.074074074074076</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>50.453720508166967</v>
+        <v>70.370370370370367</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>49.364791288566245</v>
+        <v>70.370370370370367</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>49.727767695099814</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>51.905626134301272</v>
+        <v>73.333333333333329</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>51.905626134301272</v>
+        <v>72.962962962962962</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>52.631578947368418</v>
+        <v>74.074074074074076</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>53.539019963702358</v>
+        <v>75.18518518518519</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>52.813067150635206</v>
+        <v>74.81481481481481</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>53.176043557168782</v>
+        <v>74.444444444444443</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>50.090744101633391</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>50.635208711433755</v>
+        <v>70.370370370370367</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>50.816696914700543</v>
+        <v>71.851851851851862</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>51.542649727767696</v>
+        <v>70.740740740740733</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>51.542649727767696</v>
+        <v>70.740740740740733</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>56.805807622504531</v>
+        <v>75.925925925925924</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>50.090744101633391</v>
+        <v>69.259259259259252</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>51.179673321234119</v>
+        <v>69.629629629629633</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>51.179673321234119</v>
+        <v>70.740740740740733</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>52.631578947368418</v>
+        <v>74.444444444444443</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>52.45009074410163</v>
+        <v>74.444444444444443</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>53.35753176043557</v>
+        <v>75.18518518518519</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>52.994555353901994</v>
+        <v>74.444444444444443</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>51.361161524500908</v>
+        <v>70.740740740740733</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>51.361161524500908</v>
+        <v>71.481481481481481</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>50.998185117967331</v>
+        <v>70.740740740740733</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>54.446460980036292</v>
+        <v>74.81481481481481</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>52.08711433756806</v>
+        <v>71.111111111111114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>